<commit_message>
update olahan data dan referensi tentang pupuk.
</commit_message>
<xml_diff>
--- a/HEESI/HEESI Energy Balance Update Proccessed Oct 2019.xlsx
+++ b/HEESI/HEESI Energy Balance Update Proccessed Oct 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MY JOB\2019\MEI PERBAIKAN MODEL\Model\Uji Kebijakan RPJMN\Model\Update Data Energy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\System Dynamics\system_dynamics_reference\HEESI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B80CD-57A1-411E-B0A9-531AF8B6EADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3806F0-E037-492D-817F-8ACBDE64E2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16845" yWindow="5445" windowWidth="15360" windowHeight="7620" tabRatio="676" firstSheet="15" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Balance" sheetId="15" r:id="rId1"/>
@@ -1507,19 +1507,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="13">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0000000000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2063,10 +2063,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2079,30 +2079,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -2110,7 +2110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2119,12 +2119,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2138,11 +2138,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="1" fontId="11" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2152,40 +2152,40 @@
     <xf numFmtId="1" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="11" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="15" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="15" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="13" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="13" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="13" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="13" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="15" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="13" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="13" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="13" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="15" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="15" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="14" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="14" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="14" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2289,9 +2289,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2299,7 +2299,7 @@
     <xf numFmtId="0" fontId="7" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2309,7 +2309,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2326,11 +2326,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2340,13 +2340,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2363,15 +2380,6 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2394,6 +2402,15 @@
     <xf numFmtId="0" fontId="7" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2403,14 +2420,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2451,23 +2468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2477,26 +2477,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2716,6 +2696,26 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5397,14 +5397,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{135D20DF-7485-46FA-B18F-D859BA056740}" name="Table3" displayName="Table3" ref="J5:N56" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{135D20DF-7485-46FA-B18F-D859BA056740}" name="Table3" displayName="Table3" ref="J5:N56" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="J5:N56" xr:uid="{89091FA7-F0F3-4ECB-B968-402FFBBC5C2A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E210B8D0-D5EC-4D13-B787-DE912E117C27}" name="Year" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{96E79E84-BA31-4A7B-B5C8-E3EC5FD55F56}" name="Residential" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{AE9DD58E-DD02-4996-88BA-B4EB8EF44B3B}" name="Commercial" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{7BB3D511-5C36-4424-9C04-65B3AA57F65E}" name="Industrial" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{47B338D4-C137-4959-AC03-88DC06454D51}" name="Transport" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{E210B8D0-D5EC-4D13-B787-DE912E117C27}" name="Year" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{96E79E84-BA31-4A7B-B5C8-E3EC5FD55F56}" name="Residential" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{AE9DD58E-DD02-4996-88BA-B4EB8EF44B3B}" name="Commercial" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{7BB3D511-5C36-4424-9C04-65B3AA57F65E}" name="Industrial" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{47B338D4-C137-4959-AC03-88DC06454D51}" name="Transport" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5414,7 +5414,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D4F32DF3-065F-4ADF-AD18-119A7FC25256}" name="Table14" displayName="Table14" ref="AE63:AI114" totalsRowShown="0">
   <autoFilter ref="AE63:AI114" xr:uid="{1B07480E-CEEB-4A00-A536-E6129B70621F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9E426AC0-D3BD-4FC8-986B-C15C90F56E8E}" name="Year" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{9E426AC0-D3BD-4FC8-986B-C15C90F56E8E}" name="Year" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E17068A3-556C-4EED-8D3A-04FB2F6F478B}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{E83AD156-DC29-4E59-8D79-04304071B6B6}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{8AE9B2FB-529A-49A2-A036-DDB82BE6313C}" name="Industrial"/>
@@ -5428,7 +5428,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{21AF4F1C-55CD-4065-BD3F-0251C0DC383B}" name="Table15" displayName="Table15" ref="C7:D58" totalsRowShown="0">
   <autoFilter ref="C7:D58" xr:uid="{2A4AF4E8-31FC-44A2-8485-BA91AEDAE406}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7C437757-D955-4C21-B5D5-BFB6A5EA8C16}" name="Year" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{7C437757-D955-4C21-B5D5-BFB6A5EA8C16}" name="Year" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{FBC1CA72-F6F1-4AE3-8187-27266E879D55}" name="Total Coal Primary Demand for Domestic Use "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5439,7 +5439,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{66752C7C-2B4E-472A-B171-9C5C8F2B1E64}" name="Table16" displayName="Table16" ref="G7:H58" totalsRowShown="0">
   <autoFilter ref="G7:H58" xr:uid="{633898E1-DD7B-42DF-8A92-0B3D029C0C5B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DE6B34E7-5449-4D82-AE8B-A646B87C501D}" name="Year" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{DE6B34E7-5449-4D82-AE8B-A646B87C501D}" name="Year" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{C0EE715F-0FF5-4341-8957-96EE43E8FD6C}" name="Total Petroleum Demand for Domestic Use"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5450,7 +5450,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{1C40E19A-3326-40B3-8F47-B327D0554A62}" name="Table17" displayName="Table17" ref="K7:L58" totalsRowShown="0">
   <autoFilter ref="K7:L58" xr:uid="{2E3B3821-5AAB-47CE-A79C-656BFC095771}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEAC60D7-9DE8-4B7A-9F6C-CB428068774C}" name="Year" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EEAC60D7-9DE8-4B7A-9F6C-CB428068774C}" name="Year" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{8384F11D-4F0C-42EA-BC0E-5069C7F380F6}" name="Total Gas Demand for Domestic Use"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5458,24 +5458,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E381F6A-8EB3-4457-A2F9-C2F4AE38E6BE}" name="Table4" displayName="Table4" ref="C5:G56" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E381F6A-8EB3-4457-A2F9-C2F4AE38E6BE}" name="Table4" displayName="Table4" ref="C5:G56" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="C5:G56" xr:uid="{A954B4F1-0885-44F5-AE00-63DF8167A737}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{ABEEC524-1664-451E-BD0E-2CD9C1524CD4}" name="Year" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{37745EFD-7BD7-40D2-A80D-535DD9D9ABFB}" name="Residential" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{1D64053B-928A-47C8-8F05-BFE921D40E65}" name="Commercial" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{DE70233F-60BE-491D-8D5B-CB95CB2D8221}" name="Industrial" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{1CFBC397-09B4-458C-B3EA-2BC7D301F08F}" name="Transport" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{ABEEC524-1664-451E-BD0E-2CD9C1524CD4}" name="Year" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{37745EFD-7BD7-40D2-A80D-535DD9D9ABFB}" name="Residential" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{1D64053B-928A-47C8-8F05-BFE921D40E65}" name="Commercial" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{DE70233F-60BE-491D-8D5B-CB95CB2D8221}" name="Industrial" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{1CFBC397-09B4-458C-B3EA-2BC7D301F08F}" name="Transport" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E522629F-FA93-47E9-9A3C-8AE72A4DFB71}" name="Table5" displayName="Table5" ref="Q5:U56" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E522629F-FA93-47E9-9A3C-8AE72A4DFB71}" name="Table5" displayName="Table5" ref="Q5:U56" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="Q5:U56" xr:uid="{C4215587-2F84-4984-BB7D-DFA714C003E1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A94A7EA2-F041-451B-9AFA-FBC1E379908C}" name="Year" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{A94A7EA2-F041-451B-9AFA-FBC1E379908C}" name="Year" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{B8DCEDFB-0A96-43B7-BE8E-09D0D7A21224}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{85565B56-8842-4CD9-81FD-67A7B867492F}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{9427FC23-8A34-4B5F-929F-F766D4AA59DA}" name="Industrial"/>
@@ -5486,10 +5486,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9979C5CA-79F7-4FE2-AD5E-9775F449FAED}" name="Table6" displayName="Table6" ref="AE5:AI56" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9979C5CA-79F7-4FE2-AD5E-9775F449FAED}" name="Table6" displayName="Table6" ref="AE5:AI56" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="AE5:AI56" xr:uid="{448066AA-93D6-43AD-AF79-A3028F5A5C20}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5F6E0B22-524E-442B-9DFB-491570E45C72}" name="Year" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{5F6E0B22-524E-442B-9DFB-491570E45C72}" name="Year" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{FCE3A1B6-853A-493C-A70D-3F26890FC22B}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{72035D0C-BAE8-4912-B077-6C34526D0E35}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{E6CCC93E-5B21-4FB7-8F08-4DA6D2D5F6B2}" name="Industrial"/>
@@ -5500,10 +5500,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A43927D9-284E-4F63-9B1D-97D99BD37918}" name="Table7" displayName="Table7" ref="X5:AB56" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A43927D9-284E-4F63-9B1D-97D99BD37918}" name="Table7" displayName="Table7" ref="X5:AB56" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="X5:AB56" xr:uid="{209C7562-9579-4F5E-9572-F2B02FC7E791}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0D17C27D-57F3-4753-95B0-51B01B0523C7}" name="Year" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{0D17C27D-57F3-4753-95B0-51B01B0523C7}" name="Year" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{0EBA1639-9304-4239-9448-F56E32ADBDBE}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{7696BAAC-0C4C-4871-9BD5-3574F43A427B}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{68E3C37C-0FE6-47A4-88AA-79BAC7581635}" name="Industrial"/>
@@ -5514,24 +5514,24 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{953576D6-AF3C-4C2C-8E05-10A895EA53BC}" name="Table8" displayName="Table8" ref="C63:G114" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{953576D6-AF3C-4C2C-8E05-10A895EA53BC}" name="Table8" displayName="Table8" ref="C63:G114" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="C63:G114" xr:uid="{FDE4E067-3B41-4D01-BDB5-5A6FAA64F417}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C83BB49F-E719-4D7C-B4FC-28CACE38C32C}" name="Year" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{FEF232D0-688A-4E5D-9518-9DF6688355B0}" name="Residential" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{9C95D5FF-28B6-4EF0-A668-12456E02D88E}" name="Commercial" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D2C1457C-D275-4386-BEEE-00A1BDC8CFA8}" name="Industrial" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B9FFEC1E-6E0E-4B0B-A397-7D2D84DF81AF}" name="Transport" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C83BB49F-E719-4D7C-B4FC-28CACE38C32C}" name="Year" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{FEF232D0-688A-4E5D-9518-9DF6688355B0}" name="Residential" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{9C95D5FF-28B6-4EF0-A668-12456E02D88E}" name="Commercial" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D2C1457C-D275-4386-BEEE-00A1BDC8CFA8}" name="Industrial" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{B9FFEC1E-6E0E-4B0B-A397-7D2D84DF81AF}" name="Transport" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7434DEA3-E94E-42E7-8BDA-84173F3CB372}" name="Table10" displayName="Table10" ref="J63:N114" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7434DEA3-E94E-42E7-8BDA-84173F3CB372}" name="Table10" displayName="Table10" ref="J63:N114" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="J63:N114" xr:uid="{EC2AC2A2-7E4C-4D2F-8683-FC41ACD833B5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00A5F740-CE6D-425E-9BA0-AD9807E81B15}" name="Year" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00A5F740-CE6D-425E-9BA0-AD9807E81B15}" name="Year" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{6EA17E8C-AB3E-410F-A458-E4A66185361D}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{92B073F4-76A9-46B8-B831-4F71A7390B58}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{97AE9A1F-949B-4FF9-8A62-BD182AD9C7DF}" name="Industrial"/>
@@ -5545,7 +5545,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{FC8804C7-F4AA-4C47-8373-B8EE934B7F8B}" name="Table11" displayName="Table11" ref="Q63:U114" totalsRowShown="0">
   <autoFilter ref="Q63:U114" xr:uid="{9563DE65-8D33-4F74-B24D-D0514516345E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C9AA5F4B-B5D5-4466-AD65-81539BE33B61}" name="Year" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{C9AA5F4B-B5D5-4466-AD65-81539BE33B61}" name="Year" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{AFD03046-BC20-4A5C-9477-7723B6601F19}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{9DFE7067-9FF1-44A4-B361-8721643ED35C}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{D0D21802-BDA7-4037-A2DD-6FBE186AF5A3}" name="Industrial"/>
@@ -5559,7 +5559,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{E64F5334-491E-46E9-86BC-65E578B0D26C}" name="Table13" displayName="Table13" ref="X63:AB114" totalsRowShown="0">
   <autoFilter ref="X63:AB114" xr:uid="{1174CCE2-7CF5-4F1E-BFCD-76FA58244443}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F137B178-FBF6-4575-BA5D-564E5C1624FF}" name="Year" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{F137B178-FBF6-4575-BA5D-564E5C1624FF}" name="Year" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{C332D374-3318-48E4-AEBF-CB06AEEB0FA5}" name="Residential"/>
     <tableColumn id="3" xr3:uid="{9D28ECAA-9BDA-47CE-8857-EB4A49BD9464}" name="Commercial"/>
     <tableColumn id="4" xr3:uid="{8F9217C5-E619-46E5-AE1A-AAD66A2C5D62}" name="Industrial"/>
@@ -5868,7 +5868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F4602A-109E-41B7-AA48-98F9A723A3D3}">
   <dimension ref="A3:T35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -5890,80 +5890,80 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="176" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="169" t="s">
+      <c r="D3" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="169" t="s">
+      <c r="E3" s="176" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="169" t="s">
+      <c r="F3" s="176" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="169" t="s">
+      <c r="G3" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="169" t="s">
+      <c r="H3" s="176" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="169" t="s">
+      <c r="I3" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="169" t="s">
+      <c r="J3" s="176" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="169" t="s">
+      <c r="K3" s="176" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="169" t="s">
+      <c r="L3" s="176" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="169" t="s">
+      <c r="M3" s="176" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="169" t="s">
+      <c r="N3" s="176" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="169" t="s">
+      <c r="O3" s="176" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="170" t="s">
+      <c r="P3" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="169" t="s">
+      <c r="Q3" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="169" t="s">
+      <c r="R3" s="176" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="167" t="s">
+      <c r="S3" s="177" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="168" t="s">
+      <c r="T3" s="178" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
-      <c r="H4" s="169"/>
-      <c r="I4" s="169"/>
-      <c r="J4" s="169"/>
-      <c r="K4" s="169"/>
-      <c r="L4" s="169"/>
-      <c r="M4" s="169"/>
-      <c r="N4" s="169"/>
-      <c r="O4" s="169"/>
-      <c r="P4" s="170"/>
-      <c r="Q4" s="169"/>
-      <c r="R4" s="169"/>
-      <c r="S4" s="167"/>
-      <c r="T4" s="168"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+      <c r="H4" s="176"/>
+      <c r="I4" s="176"/>
+      <c r="J4" s="176"/>
+      <c r="K4" s="176"/>
+      <c r="L4" s="176"/>
+      <c r="M4" s="176"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="176"/>
+      <c r="P4" s="179"/>
+      <c r="Q4" s="176"/>
+      <c r="R4" s="176"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="178"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -7591,6 +7591,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -7600,15 +7609,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7635,46 +7635,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="182" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="182"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="182"/>
+      <c r="N1" s="182"/>
+      <c r="O1" s="182"/>
+      <c r="P1" s="182"/>
+      <c r="Q1" s="182"/>
+      <c r="R1" s="182"/>
+      <c r="S1" s="182"/>
+      <c r="T1" s="182"/>
     </row>
     <row r="2" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182"/>
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D3">
@@ -9692,7 +9692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5ADC0A-7BD7-478A-8363-894112393048}">
   <dimension ref="B2:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>
@@ -9714,18 +9714,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
@@ -9760,7 +9760,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="176" t="s">
+      <c r="B4" s="192" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="17">
@@ -9795,7 +9795,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="176"/>
+      <c r="B5" s="192"/>
       <c r="C5" s="17">
         <v>2001</v>
       </c>
@@ -9828,7 +9828,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="176"/>
+      <c r="B6" s="192"/>
       <c r="C6" s="17">
         <v>2002</v>
       </c>
@@ -9861,7 +9861,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="176"/>
+      <c r="B7" s="192"/>
       <c r="C7" s="17">
         <v>2003</v>
       </c>
@@ -9894,7 +9894,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="176"/>
+      <c r="B8" s="192"/>
       <c r="C8" s="17">
         <v>2004</v>
       </c>
@@ -9927,7 +9927,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="176"/>
+      <c r="B9" s="192"/>
       <c r="C9" s="17">
         <v>2005</v>
       </c>
@@ -9960,7 +9960,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="176"/>
+      <c r="B10" s="192"/>
       <c r="C10" s="17">
         <v>2006</v>
       </c>
@@ -10313,18 +10313,18 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="175" t="s">
+      <c r="C23" s="191" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="175"/>
-      <c r="E23" s="175"/>
-      <c r="F23" s="175"/>
-      <c r="G23" s="175"/>
-      <c r="H23" s="175"/>
-      <c r="I23" s="175"/>
-      <c r="J23" s="175"/>
-      <c r="K23" s="175"/>
-      <c r="L23" s="175"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="191"/>
+      <c r="F23" s="191"/>
+      <c r="G23" s="191"/>
+      <c r="H23" s="191"/>
+      <c r="I23" s="191"/>
+      <c r="J23" s="191"/>
+      <c r="K23" s="191"/>
+      <c r="L23" s="191"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
@@ -10359,7 +10359,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="176" t="s">
+      <c r="B25" s="192" t="s">
         <v>129</v>
       </c>
       <c r="C25" s="17">
@@ -10403,7 +10403,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="176"/>
+      <c r="B26" s="192"/>
       <c r="C26" s="17">
         <v>2001</v>
       </c>
@@ -10445,7 +10445,7 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="176"/>
+      <c r="B27" s="192"/>
       <c r="C27" s="17">
         <v>2002</v>
       </c>
@@ -10487,7 +10487,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="176"/>
+      <c r="B28" s="192"/>
       <c r="C28" s="17">
         <v>2003</v>
       </c>
@@ -10529,7 +10529,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="176"/>
+      <c r="B29" s="192"/>
       <c r="C29" s="17">
         <v>2004</v>
       </c>
@@ -10571,7 +10571,7 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="176"/>
+      <c r="B30" s="192"/>
       <c r="C30" s="17">
         <v>2005</v>
       </c>
@@ -10613,7 +10613,7 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="176"/>
+      <c r="B31" s="192"/>
       <c r="C31" s="17">
         <v>2006</v>
       </c>
@@ -11074,17 +11074,17 @@
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D44" s="177" t="s">
+      <c r="D44" s="193" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="177"/>
-      <c r="F44" s="177"/>
-      <c r="G44" s="177"/>
-      <c r="H44" s="177"/>
-      <c r="I44" s="177"/>
-      <c r="J44" s="177"/>
-      <c r="K44" s="177"/>
-      <c r="L44" s="177"/>
+      <c r="E44" s="193"/>
+      <c r="F44" s="193"/>
+      <c r="G44" s="193"/>
+      <c r="H44" s="193"/>
+      <c r="I44" s="193"/>
+      <c r="J44" s="193"/>
+      <c r="K44" s="193"/>
+      <c r="L44" s="193"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="str">
@@ -11843,15 +11843,15 @@
       </c>
     </row>
     <row r="64" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C64" s="184" t="s">
+      <c r="C64" s="190" t="s">
         <v>477</v>
       </c>
-      <c r="D64" s="184"/>
-      <c r="E64" s="184"/>
-      <c r="F64" s="184"/>
-      <c r="G64" s="184"/>
-      <c r="H64" s="184"/>
-      <c r="I64" s="184"/>
+      <c r="D64" s="190"/>
+      <c r="E64" s="190"/>
+      <c r="F64" s="190"/>
+      <c r="G64" s="190"/>
+      <c r="H64" s="190"/>
+      <c r="I64" s="190"/>
       <c r="K64" s="4"/>
       <c r="L64" s="165" t="s">
         <v>135</v>
@@ -11973,7 +11973,7 @@
         <v>0</v>
       </c>
       <c r="E67" s="33">
-        <f t="shared" ref="E67:F82" si="16">SUM(D47)</f>
+        <f t="shared" ref="E67:E82" si="16">SUM(D47)</f>
         <v>8834.1941719999995</v>
       </c>
       <c r="F67" s="33">
@@ -12676,30 +12676,30 @@
         <f t="shared" si="20"/>
         <v>7763.568147</v>
       </c>
-      <c r="K79" s="207">
+      <c r="K79" s="170">
         <v>2013</v>
       </c>
-      <c r="L79" s="204">
+      <c r="L79" s="167">
         <f>SUM(H79,'Industrial Energy Consumption'!I82,'Domestic Energy Consumption'!P60,'Transport Energy Consumption'!Q64)</f>
         <v>703327.88406900014</v>
       </c>
-      <c r="M79" s="204">
+      <c r="M79" s="167">
         <f>SUM(D79,'Industrial Energy Consumption'!E82)</f>
         <v>262205.49031700002</v>
       </c>
-      <c r="N79" s="204">
+      <c r="N79" s="167">
         <f>SUM(E79,'Industrial Energy Consumption'!F82,'Domestic Energy Consumption'!M60,'Transport Energy Consumption'!P64)</f>
         <v>2282648.0996560003</v>
       </c>
-      <c r="O79" s="204">
+      <c r="O79" s="167">
         <f>SUM(F119,'Industrial Energy Consumption'!G82,'Domestic Energy Consumption'!N60,'Transport Energy Consumption'!N64)</f>
         <v>1068172.7619370001</v>
       </c>
-      <c r="P79" s="204">
+      <c r="P79" s="167">
         <f>SUM(G79,'Industrial Energy Consumption'!H82,'Domestic Energy Consumption'!O60,'Other Energy Consumption'!S43,'Transport Energy Consumption'!O64)</f>
         <v>2717597.5696410006</v>
       </c>
-      <c r="Q79" s="204">
+      <c r="Q79" s="167">
         <f t="shared" si="21"/>
         <v>7033951.8056200007</v>
       </c>
@@ -12879,21 +12879,21 @@
       <c r="K83" s="164"/>
     </row>
     <row r="84" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C84" s="178" t="s">
+      <c r="C84" s="184" t="s">
         <v>138</v>
       </c>
-      <c r="D84" s="179"/>
-      <c r="E84" s="179"/>
-      <c r="F84" s="179"/>
-      <c r="G84" s="179"/>
-      <c r="H84" s="179"/>
-      <c r="I84" s="180"/>
-      <c r="L84" s="209"/>
-      <c r="M84" s="209"/>
-      <c r="N84" s="209"/>
-      <c r="O84" s="209"/>
-      <c r="P84" s="209"/>
-      <c r="Q84" s="209"/>
+      <c r="D84" s="185"/>
+      <c r="E84" s="185"/>
+      <c r="F84" s="185"/>
+      <c r="G84" s="185"/>
+      <c r="H84" s="185"/>
+      <c r="I84" s="186"/>
+      <c r="L84" s="172"/>
+      <c r="M84" s="172"/>
+      <c r="N84" s="172"/>
+      <c r="O84" s="172"/>
+      <c r="P84" s="172"/>
+      <c r="Q84" s="172"/>
     </row>
     <row r="85" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C85" s="152" t="s">
@@ -12917,12 +12917,12 @@
       <c r="I85" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="L85" s="210"/>
-      <c r="M85" s="211"/>
-      <c r="N85" s="211"/>
-      <c r="O85" s="211"/>
-      <c r="P85" s="211"/>
-      <c r="Q85" s="211"/>
+      <c r="L85" s="173"/>
+      <c r="M85" s="174"/>
+      <c r="N85" s="174"/>
+      <c r="O85" s="174"/>
+      <c r="P85" s="174"/>
+      <c r="Q85" s="174"/>
     </row>
     <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C86" s="142">
@@ -12947,12 +12947,12 @@
         <f>SUM(D86:H86)</f>
         <v>178733.27990000002</v>
       </c>
-      <c r="L86" s="212"/>
-      <c r="M86" s="212"/>
-      <c r="N86" s="212"/>
-      <c r="O86" s="212"/>
-      <c r="P86" s="212"/>
-      <c r="Q86" s="212"/>
+      <c r="L86" s="175"/>
+      <c r="M86" s="175"/>
+      <c r="N86" s="175"/>
+      <c r="O86" s="175"/>
+      <c r="P86" s="175"/>
+      <c r="Q86" s="175"/>
     </row>
     <row r="87" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C87" s="142">
@@ -12974,7 +12974,7 @@
         <v>26251.737260000002</v>
       </c>
       <c r="I87" s="144">
-        <f t="shared" ref="I87:I103" si="22">SUM(D87:H87)</f>
+        <f t="shared" ref="I87:I102" si="22">SUM(D87:H87)</f>
         <v>187114.7481</v>
       </c>
       <c r="L87" s="35"/>
@@ -13354,15 +13354,15 @@
       <c r="I103" s="144"/>
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C104" s="181" t="s">
+      <c r="C104" s="187" t="s">
         <v>478</v>
       </c>
-      <c r="D104" s="182"/>
-      <c r="E104" s="182"/>
-      <c r="F104" s="182"/>
-      <c r="G104" s="182"/>
-      <c r="H104" s="182"/>
-      <c r="I104" s="183"/>
+      <c r="D104" s="188"/>
+      <c r="E104" s="188"/>
+      <c r="F104" s="188"/>
+      <c r="G104" s="188"/>
+      <c r="H104" s="188"/>
+      <c r="I104" s="189"/>
     </row>
     <row r="105" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C105" s="153" t="s">
@@ -13397,15 +13397,15 @@
         <f>SUM(E66)</f>
         <v>8883.1370760000009</v>
       </c>
-      <c r="F106" s="208">
+      <c r="F106" s="171">
         <f>SUM(F66,I66)</f>
         <v>16200.101224000002</v>
       </c>
-      <c r="G106" s="208">
+      <c r="G106" s="171">
         <f>G66+I86</f>
         <v>233096.61051800003</v>
       </c>
-      <c r="H106" s="208">
+      <c r="H106" s="171">
         <f>H66</f>
         <v>54712.048809</v>
       </c>
@@ -13423,16 +13423,16 @@
         <f t="shared" si="23"/>
         <v>8834.1941719999995</v>
       </c>
-      <c r="F107" s="208">
+      <c r="F107" s="171">
         <f t="shared" ref="F107:F122" si="24">SUM(F67,I67)</f>
         <v>14823.582049000001</v>
       </c>
-      <c r="G107" s="208">
+      <c r="G107" s="171">
         <f t="shared" ref="G107:G122" si="25">G67+I87</f>
         <v>243197.198221</v>
       </c>
-      <c r="H107" s="208">
-        <f t="shared" ref="H107:I107" si="26">H67</f>
+      <c r="H107" s="171">
+        <f t="shared" ref="H107" si="26">H67</f>
         <v>58456.180965</v>
       </c>
       <c r="I107" s="154"/>
@@ -13449,16 +13449,16 @@
         <f t="shared" si="27"/>
         <v>8791.3691310000013</v>
       </c>
-      <c r="F108" s="208">
+      <c r="F108" s="171">
         <f t="shared" si="24"/>
         <v>16652.823086</v>
       </c>
-      <c r="G108" s="208">
+      <c r="G108" s="171">
         <f t="shared" si="25"/>
         <v>237984.78070599999</v>
       </c>
-      <c r="H108" s="208">
-        <f t="shared" ref="H108:I108" si="28">H68</f>
+      <c r="H108" s="171">
+        <f t="shared" ref="H108" si="28">H68</f>
         <v>60995.094110000005</v>
       </c>
       <c r="I108" s="154"/>
@@ -13475,16 +13475,16 @@
         <f t="shared" si="29"/>
         <v>8748.5440900000012</v>
       </c>
-      <c r="F109" s="208">
+      <c r="F109" s="171">
         <f t="shared" si="24"/>
         <v>12541.619150000002</v>
       </c>
-      <c r="G109" s="208">
+      <c r="G109" s="171">
         <f t="shared" si="25"/>
         <v>228428.68281600002</v>
       </c>
-      <c r="H109" s="208">
-        <f t="shared" ref="H109:I109" si="30">H69</f>
+      <c r="H109" s="171">
+        <f t="shared" ref="H109" si="30">H69</f>
         <v>68220.290313000005</v>
       </c>
       <c r="I109" s="154"/>
@@ -13501,16 +13501,16 @@
         <f t="shared" si="31"/>
         <v>8705.7190490000012</v>
       </c>
-      <c r="F110" s="208">
+      <c r="F110" s="171">
         <f t="shared" si="24"/>
         <v>16824.123250000001</v>
       </c>
-      <c r="G110" s="208">
+      <c r="G110" s="171">
         <f t="shared" si="25"/>
         <v>252233.27856000004</v>
       </c>
-      <c r="H110" s="208">
-        <f t="shared" ref="H110:I110" si="32">H70</f>
+      <c r="H110" s="171">
+        <f t="shared" ref="H110" si="32">H70</f>
         <v>79446.568918000004</v>
       </c>
       <c r="I110" s="154"/>
@@ -13527,16 +13527,16 @@
         <f t="shared" si="33"/>
         <v>8662.8940080000011</v>
       </c>
-      <c r="F111" s="208">
+      <c r="F111" s="171">
         <f t="shared" si="24"/>
         <v>17362.495193999999</v>
       </c>
-      <c r="G111" s="208">
+      <c r="G111" s="171">
         <f t="shared" si="25"/>
         <v>240064.85328300003</v>
       </c>
-      <c r="H111" s="208">
-        <f t="shared" ref="H111:I111" si="34">H71</f>
+      <c r="H111" s="171">
+        <f t="shared" ref="H111" si="34">H71</f>
         <v>87754.626872000008</v>
       </c>
       <c r="I111" s="154"/>
@@ -13553,16 +13553,16 @@
         <f t="shared" si="35"/>
         <v>8620.0689670000011</v>
       </c>
-      <c r="F112" s="208">
+      <c r="F112" s="171">
         <f t="shared" si="24"/>
         <v>16444.815744000003</v>
       </c>
-      <c r="G112" s="208">
+      <c r="G112" s="171">
         <f t="shared" si="25"/>
         <v>214687.966721</v>
       </c>
-      <c r="H112" s="208">
-        <f t="shared" ref="H112:I112" si="36">H72</f>
+      <c r="H112" s="171">
+        <f t="shared" ref="H112" si="36">H72</f>
         <v>94661.694199000005</v>
       </c>
       <c r="I112" s="154"/>
@@ -13579,16 +13579,16 @@
         <f t="shared" si="37"/>
         <v>8577.243926000001</v>
       </c>
-      <c r="F113" s="208">
+      <c r="F113" s="171">
         <f t="shared" si="24"/>
         <v>17680.624069999998</v>
       </c>
-      <c r="G113" s="208">
+      <c r="G113" s="171">
         <f t="shared" si="25"/>
         <v>197925.02791800001</v>
       </c>
-      <c r="H113" s="208">
-        <f t="shared" ref="H113:I113" si="38">H73</f>
+      <c r="H113" s="171">
+        <f t="shared" ref="H113" si="38">H73</f>
         <v>105135.475655</v>
       </c>
       <c r="I113" s="154"/>
@@ -13605,16 +13605,16 @@
         <f t="shared" si="39"/>
         <v>8534.418885000001</v>
       </c>
-      <c r="F114" s="208">
+      <c r="F114" s="171">
         <f t="shared" si="24"/>
         <v>14958.175035</v>
       </c>
-      <c r="G114" s="208">
+      <c r="G114" s="171">
         <f t="shared" si="25"/>
         <v>193452.870716</v>
       </c>
-      <c r="H114" s="208">
-        <f t="shared" ref="H114:I114" si="40">H74</f>
+      <c r="H114" s="171">
+        <f t="shared" ref="H114" si="40">H74</f>
         <v>115450.19267300001</v>
       </c>
       <c r="I114" s="154"/>
@@ -13631,16 +13631,16 @@
         <f t="shared" si="41"/>
         <v>8491.5938440000009</v>
       </c>
-      <c r="F115" s="208">
+      <c r="F115" s="171">
         <f t="shared" si="24"/>
         <v>17056.602043999999</v>
       </c>
-      <c r="G115" s="208">
+      <c r="G115" s="171">
         <f t="shared" si="25"/>
         <v>191348.32517500001</v>
       </c>
-      <c r="H115" s="208">
-        <f t="shared" ref="H115:I115" si="42">H75</f>
+      <c r="H115" s="171">
+        <f t="shared" ref="H115" si="42">H75</f>
         <v>124963.46963800001</v>
       </c>
       <c r="I115" s="154"/>
@@ -13657,16 +13657,16 @@
         <f t="shared" si="43"/>
         <v>8448.7688030000008</v>
       </c>
-      <c r="F116" s="208">
+      <c r="F116" s="171">
         <f t="shared" si="24"/>
         <v>18445.356945</v>
       </c>
-      <c r="G116" s="208">
+      <c r="G116" s="171">
         <f t="shared" si="25"/>
         <v>166277.33145700002</v>
       </c>
-      <c r="H116" s="208">
-        <f t="shared" ref="H116:I116" si="44">H76</f>
+      <c r="H116" s="171">
+        <f t="shared" ref="H116" si="44">H76</f>
         <v>139034.554538</v>
       </c>
       <c r="I116" s="154"/>
@@ -13683,16 +13683,16 @@
         <f t="shared" si="45"/>
         <v>8405.9437620000008</v>
       </c>
-      <c r="F117" s="208">
+      <c r="F117" s="171">
         <f t="shared" si="24"/>
         <v>21498.170581999999</v>
       </c>
-      <c r="G117" s="208">
+      <c r="G117" s="171">
         <f t="shared" si="25"/>
         <v>202446.12287300001</v>
       </c>
-      <c r="H117" s="208">
-        <f t="shared" ref="H117:I117" si="46">H77</f>
+      <c r="H117" s="171">
+        <f t="shared" ref="H117" si="46">H77</f>
         <v>156819.182279</v>
       </c>
       <c r="I117" s="154"/>
@@ -13709,16 +13709,16 @@
         <f t="shared" si="47"/>
         <v>8363.1187210000007</v>
       </c>
-      <c r="F118" s="208">
+      <c r="F118" s="171">
         <f t="shared" si="24"/>
         <v>23878.019289</v>
       </c>
-      <c r="G118" s="208">
+      <c r="G118" s="171">
         <f t="shared" si="25"/>
         <v>252239.39035999999</v>
       </c>
-      <c r="H118" s="208">
-        <f t="shared" ref="H118:I118" si="48">H78</f>
+      <c r="H118" s="171">
+        <f t="shared" ref="H118" si="48">H78</f>
         <v>155913.73855500002</v>
       </c>
       <c r="I118" s="154"/>
@@ -13735,16 +13735,16 @@
         <f t="shared" si="49"/>
         <v>8320.2936800000007</v>
       </c>
-      <c r="F119" s="208">
+      <c r="F119" s="171">
         <f t="shared" si="24"/>
         <v>24226.737479999996</v>
       </c>
-      <c r="G119" s="208">
+      <c r="G119" s="171">
         <f t="shared" si="25"/>
         <v>233708.39115099999</v>
       </c>
-      <c r="H119" s="208">
-        <f t="shared" ref="H119:I119" si="50">H79</f>
+      <c r="H119" s="171">
+        <f t="shared" ref="H119" si="50">H79</f>
         <v>171838.535944</v>
       </c>
       <c r="I119" s="154"/>
@@ -13761,16 +13761,16 @@
         <f t="shared" si="51"/>
         <v>8277.4686390000006</v>
       </c>
-      <c r="F120" s="208">
+      <c r="F120" s="171">
         <f t="shared" si="24"/>
         <v>25725.613915000002</v>
       </c>
-      <c r="G120" s="208">
+      <c r="G120" s="171">
         <f t="shared" si="25"/>
         <v>214510.54428700003</v>
       </c>
-      <c r="H120" s="208">
-        <f t="shared" ref="H120:I120" si="52">H80</f>
+      <c r="H120" s="171">
+        <f t="shared" ref="H120" si="52">H80</f>
         <v>181706.64896300001</v>
       </c>
       <c r="I120" s="154"/>
@@ -13787,16 +13787,16 @@
         <f t="shared" si="53"/>
         <v>8234.6435980000006</v>
       </c>
-      <c r="F121" s="208">
+      <c r="F121" s="171">
         <f t="shared" si="24"/>
         <v>26447.521749</v>
       </c>
-      <c r="G121" s="208">
+      <c r="G121" s="171">
         <f t="shared" si="25"/>
         <v>247663.23145800002</v>
       </c>
-      <c r="H121" s="208">
-        <f t="shared" ref="H121:I121" si="54">H81</f>
+      <c r="H121" s="171">
+        <f t="shared" ref="H121" si="54">H81</f>
         <v>187059.77908800001</v>
       </c>
       <c r="I121" s="154"/>
@@ -13813,30 +13813,30 @@
         <f t="shared" si="55"/>
         <v>8197.93642</v>
       </c>
-      <c r="F122" s="208">
+      <c r="F122" s="171">
         <f t="shared" si="24"/>
         <v>26184.45364</v>
       </c>
-      <c r="G122" s="208">
+      <c r="G122" s="171">
         <f t="shared" si="25"/>
         <v>144828.112479</v>
       </c>
-      <c r="H122" s="208">
-        <f t="shared" ref="H122:I122" si="56">H82</f>
+      <c r="H122" s="171">
+        <f t="shared" ref="H122" si="56">H82</f>
         <v>202519.618889</v>
       </c>
       <c r="I122" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="D44:L44"/>
     <mergeCell ref="C84:I84"/>
     <mergeCell ref="C104:I104"/>
     <mergeCell ref="C64:I64"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C23:L23"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="D44:L44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13872,15 +13872,15 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="175" t="s">
+      <c r="C4" s="191" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="175"/>
-      <c r="G4" s="175"/>
-      <c r="H4" s="175"/>
-      <c r="I4" s="175"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="191"/>
+      <c r="I4" s="191"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
@@ -13912,7 +13912,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="192" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="17">
@@ -13946,7 +13946,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="176"/>
+      <c r="B7" s="192"/>
       <c r="C7" s="17">
         <v>2001</v>
       </c>
@@ -13978,7 +13978,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="176"/>
+      <c r="B8" s="192"/>
       <c r="C8" s="17">
         <v>2002</v>
       </c>
@@ -14010,7 +14010,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="176"/>
+      <c r="B9" s="192"/>
       <c r="C9" s="17">
         <v>2003</v>
       </c>
@@ -14042,7 +14042,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="176"/>
+      <c r="B10" s="192"/>
       <c r="C10" s="17">
         <v>2004</v>
       </c>
@@ -14074,7 +14074,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="176"/>
+      <c r="B11" s="192"/>
       <c r="C11" s="17">
         <v>2005</v>
       </c>
@@ -14106,7 +14106,7 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="176"/>
+      <c r="B12" s="192"/>
       <c r="C12" s="17">
         <v>2006</v>
       </c>
@@ -14448,30 +14448,30 @@
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C24" s="175" t="s">
+      <c r="C24" s="191" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="175"/>
-      <c r="E24" s="175"/>
-      <c r="F24" s="175"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="175"/>
-      <c r="I24" s="175"/>
+      <c r="D24" s="191"/>
+      <c r="E24" s="191"/>
+      <c r="F24" s="191"/>
+      <c r="G24" s="191"/>
+      <c r="H24" s="191"/>
+      <c r="I24" s="191"/>
       <c r="L24" t="s">
         <v>130</v>
       </c>
       <c r="M24">
         <v>6.1178600000000001E-3</v>
       </c>
-      <c r="N24" s="175" t="s">
+      <c r="N24" s="191" t="s">
         <v>136</v>
       </c>
-      <c r="O24" s="175"/>
-      <c r="P24" s="175"/>
-      <c r="Q24" s="175"/>
-      <c r="R24" s="175"/>
-      <c r="S24" s="175"/>
-      <c r="T24" s="175"/>
+      <c r="O24" s="191"/>
+      <c r="P24" s="191"/>
+      <c r="Q24" s="191"/>
+      <c r="R24" s="191"/>
+      <c r="S24" s="191"/>
+      <c r="T24" s="191"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
@@ -14539,7 +14539,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="176" t="s">
+      <c r="B26" s="192" t="s">
         <v>129</v>
       </c>
       <c r="C26" s="17">
@@ -14616,7 +14616,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="176"/>
+      <c r="B27" s="192"/>
       <c r="C27" s="17">
         <f t="shared" si="5"/>
         <v>2001</v>
@@ -14691,7 +14691,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="176"/>
+      <c r="B28" s="192"/>
       <c r="C28" s="17">
         <f t="shared" si="5"/>
         <v>2002</v>
@@ -14766,7 +14766,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="176"/>
+      <c r="B29" s="192"/>
       <c r="C29" s="17">
         <f t="shared" si="5"/>
         <v>2003</v>
@@ -14841,7 +14841,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="176"/>
+      <c r="B30" s="192"/>
       <c r="C30" s="17">
         <f t="shared" si="5"/>
         <v>2004</v>
@@ -14916,7 +14916,7 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="176"/>
+      <c r="B31" s="192"/>
       <c r="C31" s="17">
         <f t="shared" si="5"/>
         <v>2005</v>
@@ -14991,7 +14991,7 @@
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="176"/>
+      <c r="B32" s="192"/>
       <c r="C32" s="17">
         <f>C33-1</f>
         <v>2006</v>
@@ -15796,14 +15796,14 @@
       </c>
     </row>
     <row r="44" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="N44" s="185" t="s">
+      <c r="N44" s="194" t="s">
         <v>136</v>
       </c>
-      <c r="O44" s="186"/>
-      <c r="P44" s="186"/>
-      <c r="Q44" s="186"/>
-      <c r="R44" s="186"/>
-      <c r="S44" s="187"/>
+      <c r="O44" s="195"/>
+      <c r="P44" s="195"/>
+      <c r="Q44" s="195"/>
+      <c r="R44" s="195"/>
+      <c r="S44" s="196"/>
       <c r="T44" s="36"/>
     </row>
     <row r="45" spans="3:22" x14ac:dyDescent="0.25">
@@ -16262,22 +16262,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="188" t="s">
+      <c r="D2" s="198" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
-      <c r="K2" s="188"/>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="188"/>
-      <c r="P2" s="188"/>
-      <c r="Q2" s="188"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
       <c r="S2" t="s">
         <v>480</v>
       </c>
@@ -16335,7 +16335,7 @@
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="176" t="s">
+      <c r="C4" s="192" t="s">
         <v>129</v>
       </c>
       <c r="D4" s="17">
@@ -16391,7 +16391,7 @@
       </c>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C5" s="176"/>
+      <c r="C5" s="192"/>
       <c r="D5" s="17">
         <f t="shared" si="0"/>
         <v>2001</v>
@@ -16445,7 +16445,7 @@
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C6" s="176"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -16499,7 +16499,7 @@
       </c>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="176"/>
+      <c r="C7" s="192"/>
       <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -16553,7 +16553,7 @@
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C8" s="176"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="17">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -16607,7 +16607,7 @@
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="176"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="17">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -16661,7 +16661,7 @@
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="176"/>
+      <c r="C10" s="192"/>
       <c r="D10" s="17">
         <f>D11-1</f>
         <v>2006</v>
@@ -17231,22 +17231,22 @@
       </c>
     </row>
     <row r="24" spans="3:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D24" s="188" t="s">
+      <c r="D24" s="198" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="188"/>
-      <c r="F24" s="188"/>
-      <c r="G24" s="188"/>
-      <c r="H24" s="188"/>
-      <c r="I24" s="188"/>
-      <c r="J24" s="188"/>
-      <c r="K24" s="188"/>
-      <c r="L24" s="188"/>
-      <c r="M24" s="188"/>
-      <c r="N24" s="188"/>
-      <c r="O24" s="188"/>
-      <c r="P24" s="188"/>
-      <c r="Q24" s="188"/>
+      <c r="E24" s="198"/>
+      <c r="F24" s="198"/>
+      <c r="G24" s="198"/>
+      <c r="H24" s="198"/>
+      <c r="I24" s="198"/>
+      <c r="J24" s="198"/>
+      <c r="K24" s="198"/>
+      <c r="L24" s="198"/>
+      <c r="M24" s="198"/>
+      <c r="N24" s="198"/>
+      <c r="O24" s="198"/>
+      <c r="P24" s="198"/>
+      <c r="Q24" s="198"/>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
@@ -17302,7 +17302,7 @@
       </c>
     </row>
     <row r="26" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C26" s="176" t="s">
+      <c r="C26" s="192" t="s">
         <v>129</v>
       </c>
       <c r="D26" s="17">
@@ -17373,12 +17373,12 @@
         <f t="shared" ref="T26:T32" si="6">S26/1000000</f>
         <v>233.30799999999999</v>
       </c>
-      <c r="U26" s="190" t="s">
+      <c r="U26" s="197" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="27" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C27" s="176"/>
+      <c r="C27" s="192"/>
       <c r="D27" s="17">
         <f t="shared" si="2"/>
         <v>2001</v>
@@ -17447,10 +17447,10 @@
         <f t="shared" si="6"/>
         <v>245.49700000000001</v>
       </c>
-      <c r="U27" s="190"/>
+      <c r="U27" s="197"/>
     </row>
     <row r="28" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C28" s="176"/>
+      <c r="C28" s="192"/>
       <c r="D28" s="17">
         <f t="shared" si="2"/>
         <v>2002</v>
@@ -17519,10 +17519,10 @@
         <f t="shared" si="6"/>
         <v>241.33799999999999</v>
       </c>
-      <c r="U28" s="190"/>
+      <c r="U28" s="197"/>
     </row>
     <row r="29" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C29" s="176"/>
+      <c r="C29" s="192"/>
       <c r="D29" s="17">
         <f t="shared" si="2"/>
         <v>2003</v>
@@ -17591,10 +17591,10 @@
         <f t="shared" si="6"/>
         <v>273.459</v>
       </c>
-      <c r="U29" s="190"/>
+      <c r="U29" s="197"/>
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C30" s="176"/>
+      <c r="C30" s="192"/>
       <c r="D30" s="17">
         <f t="shared" si="2"/>
         <v>2004</v>
@@ -17663,10 +17663,10 @@
         <f t="shared" si="6"/>
         <v>278.75299999999999</v>
       </c>
-      <c r="U30" s="190"/>
+      <c r="U30" s="197"/>
     </row>
     <row r="31" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C31" s="176"/>
+      <c r="C31" s="192"/>
       <c r="D31" s="17">
         <f t="shared" si="2"/>
         <v>2005</v>
@@ -17735,10 +17735,10 @@
         <f t="shared" si="6"/>
         <v>273.12</v>
       </c>
-      <c r="U31" s="190"/>
+      <c r="U31" s="197"/>
     </row>
     <row r="32" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C32" s="176"/>
+      <c r="C32" s="192"/>
       <c r="D32" s="17">
         <f>D33-1</f>
         <v>2006</v>
@@ -17807,7 +17807,7 @@
         <f t="shared" si="6"/>
         <v>298.50200000000001</v>
       </c>
-      <c r="U32" s="190"/>
+      <c r="U32" s="197"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D33" s="4">
@@ -18512,22 +18512,22 @@
       <c r="F46" s="31"/>
     </row>
     <row r="47" spans="3:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D47" s="188" t="s">
+      <c r="D47" s="198" t="s">
         <v>134</v>
       </c>
-      <c r="E47" s="188"/>
-      <c r="F47" s="188"/>
-      <c r="G47" s="188"/>
-      <c r="H47" s="188"/>
-      <c r="I47" s="188"/>
-      <c r="J47" s="188"/>
-      <c r="K47" s="188"/>
-      <c r="L47" s="188"/>
-      <c r="M47" s="188"/>
-      <c r="N47" s="188"/>
-      <c r="O47" s="188"/>
-      <c r="P47" s="188"/>
-      <c r="Q47" s="188"/>
+      <c r="E47" s="198"/>
+      <c r="F47" s="198"/>
+      <c r="G47" s="198"/>
+      <c r="H47" s="198"/>
+      <c r="I47" s="198"/>
+      <c r="J47" s="198"/>
+      <c r="K47" s="198"/>
+      <c r="L47" s="198"/>
+      <c r="M47" s="198"/>
+      <c r="N47" s="198"/>
+      <c r="O47" s="198"/>
+      <c r="P47" s="198"/>
+      <c r="Q47" s="198"/>
     </row>
     <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D48" s="34" t="str">
@@ -19574,14 +19574,14 @@
       </c>
     </row>
     <row r="67" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D67" s="189" t="s">
+      <c r="D67" s="199" t="s">
         <v>135</v>
       </c>
-      <c r="E67" s="189"/>
-      <c r="F67" s="189"/>
-      <c r="G67" s="189"/>
-      <c r="H67" s="189"/>
-      <c r="I67" s="189"/>
+      <c r="E67" s="199"/>
+      <c r="F67" s="199"/>
+      <c r="G67" s="199"/>
+      <c r="H67" s="199"/>
+      <c r="I67" s="199"/>
     </row>
     <row r="68" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D68" s="34" t="str">
@@ -20048,13 +20048,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D24:Q24"/>
     <mergeCell ref="U26:U32"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="C26:C32"/>
     <mergeCell ref="D47:Q47"/>
     <mergeCell ref="D67:I67"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D24:Q24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -20086,15 +20086,15 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="175" t="s">
+      <c r="C4" s="191" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="175"/>
-      <c r="G4" s="175"/>
-      <c r="H4" s="175"/>
-      <c r="I4" s="175"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="191"/>
+      <c r="I4" s="191"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
@@ -20519,24 +20519,24 @@
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="175" t="s">
+      <c r="C25" s="191" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="175"/>
-      <c r="E25" s="175"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="175"/>
-      <c r="I25" s="175"/>
-      <c r="L25" s="175" t="s">
+      <c r="D25" s="191"/>
+      <c r="E25" s="191"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="191"/>
+      <c r="H25" s="191"/>
+      <c r="I25" s="191"/>
+      <c r="L25" s="191" t="s">
         <v>139</v>
       </c>
-      <c r="M25" s="175"/>
-      <c r="N25" s="175"/>
-      <c r="O25" s="175"/>
-      <c r="P25" s="175"/>
-      <c r="Q25" s="175"/>
-      <c r="R25" s="175"/>
+      <c r="M25" s="191"/>
+      <c r="N25" s="191"/>
+      <c r="O25" s="191"/>
+      <c r="P25" s="191"/>
+      <c r="Q25" s="191"/>
+      <c r="R25" s="191"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
@@ -21677,13 +21677,13 @@
       </c>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="L45" s="175" t="s">
+      <c r="L45" s="191" t="s">
         <v>139</v>
       </c>
-      <c r="M45" s="175"/>
-      <c r="N45" s="175"/>
-      <c r="O45" s="175"/>
-      <c r="P45" s="175"/>
+      <c r="M45" s="191"/>
+      <c r="N45" s="191"/>
+      <c r="O45" s="191"/>
+      <c r="P45" s="191"/>
       <c r="Q45" s="36"/>
       <c r="R45" s="36"/>
     </row>
@@ -22091,15 +22091,15 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="191" t="s">
+      <c r="D7" s="200" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="191"/>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="200"/>
+      <c r="J7" s="200"/>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" s="143" t="s">
@@ -22541,24 +22541,24 @@
       </c>
     </row>
     <row r="28" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D28" s="191" t="s">
+      <c r="D28" s="200" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="191"/>
-      <c r="F28" s="191"/>
-      <c r="G28" s="191"/>
-      <c r="H28" s="191"/>
-      <c r="I28" s="191"/>
-      <c r="J28" s="191"/>
-      <c r="M28" s="175" t="s">
+      <c r="E28" s="200"/>
+      <c r="F28" s="200"/>
+      <c r="G28" s="200"/>
+      <c r="H28" s="200"/>
+      <c r="I28" s="200"/>
+      <c r="J28" s="200"/>
+      <c r="M28" s="191" t="s">
         <v>138</v>
       </c>
-      <c r="N28" s="175"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="175"/>
-      <c r="Q28" s="175"/>
-      <c r="R28" s="175"/>
-      <c r="S28" s="175"/>
+      <c r="N28" s="191"/>
+      <c r="O28" s="191"/>
+      <c r="P28" s="191"/>
+      <c r="Q28" s="191"/>
+      <c r="R28" s="191"/>
+      <c r="S28" s="191"/>
     </row>
     <row r="29" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D29" s="143" t="s">
@@ -23603,28 +23603,28 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="194" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="186"/>
-      <c r="F5" s="186"/>
-      <c r="G5" s="186"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="186"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="186"/>
-      <c r="M5" s="186"/>
-      <c r="N5" s="186"/>
-      <c r="O5" s="186"/>
-      <c r="P5" s="186"/>
-      <c r="Q5" s="186"/>
-      <c r="R5" s="186"/>
-      <c r="S5" s="186"/>
-      <c r="T5" s="186"/>
-      <c r="U5" s="186"/>
-      <c r="V5" s="186"/>
-      <c r="W5" s="187"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="195"/>
+      <c r="G5" s="195"/>
+      <c r="H5" s="195"/>
+      <c r="I5" s="195"/>
+      <c r="J5" s="195"/>
+      <c r="K5" s="195"/>
+      <c r="L5" s="195"/>
+      <c r="M5" s="195"/>
+      <c r="N5" s="195"/>
+      <c r="O5" s="195"/>
+      <c r="P5" s="195"/>
+      <c r="Q5" s="195"/>
+      <c r="R5" s="195"/>
+      <c r="S5" s="195"/>
+      <c r="T5" s="195"/>
+      <c r="U5" s="195"/>
+      <c r="V5" s="195"/>
+      <c r="W5" s="196"/>
     </row>
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
@@ -24750,28 +24750,28 @@
       </c>
     </row>
     <row r="27" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D27" s="185" t="s">
+      <c r="D27" s="194" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="186"/>
-      <c r="F27" s="186"/>
-      <c r="G27" s="186"/>
-      <c r="H27" s="186"/>
-      <c r="I27" s="186"/>
-      <c r="J27" s="186"/>
-      <c r="K27" s="186"/>
-      <c r="L27" s="186"/>
-      <c r="M27" s="186"/>
-      <c r="N27" s="186"/>
-      <c r="O27" s="186"/>
-      <c r="P27" s="186"/>
-      <c r="Q27" s="186"/>
-      <c r="R27" s="186"/>
-      <c r="S27" s="186"/>
-      <c r="T27" s="186"/>
-      <c r="U27" s="186"/>
-      <c r="V27" s="186"/>
-      <c r="W27" s="187"/>
+      <c r="E27" s="195"/>
+      <c r="F27" s="195"/>
+      <c r="G27" s="195"/>
+      <c r="H27" s="195"/>
+      <c r="I27" s="195"/>
+      <c r="J27" s="195"/>
+      <c r="K27" s="195"/>
+      <c r="L27" s="195"/>
+      <c r="M27" s="195"/>
+      <c r="N27" s="195"/>
+      <c r="O27" s="195"/>
+      <c r="P27" s="195"/>
+      <c r="Q27" s="195"/>
+      <c r="R27" s="195"/>
+      <c r="S27" s="195"/>
+      <c r="T27" s="195"/>
+      <c r="U27" s="195"/>
+      <c r="V27" s="195"/>
+      <c r="W27" s="196"/>
     </row>
     <row r="28" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D28" s="4" t="s">
@@ -24922,7 +24922,7 @@
         <f t="shared" ref="X29:X35" si="3">W29/1000000</f>
         <v>0</v>
       </c>
-      <c r="Z29" s="205">
+      <c r="Z29" s="168">
         <f>SUM(F29:Q29)</f>
         <v>138979000</v>
       </c>
@@ -26291,27 +26291,27 @@
       <c r="C47" t="s">
         <v>474</v>
       </c>
-      <c r="D47" s="206">
+      <c r="D47" s="169">
         <v>6.1178630000000003E-3</v>
       </c>
     </row>
     <row r="49" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D49" s="192" t="s">
+      <c r="D49" s="201" t="s">
         <v>62</v>
       </c>
-      <c r="E49" s="192"/>
-      <c r="F49" s="192"/>
-      <c r="G49" s="192"/>
-      <c r="H49" s="192"/>
-      <c r="I49" s="192"/>
-      <c r="M49" s="192" t="s">
+      <c r="E49" s="201"/>
+      <c r="F49" s="201"/>
+      <c r="G49" s="201"/>
+      <c r="H49" s="201"/>
+      <c r="I49" s="201"/>
+      <c r="M49" s="201" t="s">
         <v>475</v>
       </c>
-      <c r="N49" s="192"/>
-      <c r="O49" s="192"/>
-      <c r="P49" s="192"/>
-      <c r="Q49" s="192"/>
-      <c r="R49" s="192"/>
+      <c r="N49" s="201"/>
+      <c r="O49" s="201"/>
+      <c r="P49" s="201"/>
+      <c r="Q49" s="201"/>
+      <c r="R49" s="201"/>
       <c r="S49" s="148"/>
       <c r="T49" s="148"/>
       <c r="U49" s="148"/>
@@ -27277,8 +27277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B79CA5-D6C7-4742-8B39-281C77C14FBC}">
   <dimension ref="A1:AZ257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39073,7 +39073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04907A75-0974-4B8E-AAA5-BC03EE69F478}">
   <dimension ref="C3:AI120"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T31" sqref="F26:T31"/>
     </sheetView>
   </sheetViews>
@@ -39124,36 +39124,36 @@
       </c>
     </row>
     <row r="4" spans="3:35" x14ac:dyDescent="0.25">
-      <c r="D4" s="198" t="s">
+      <c r="D4" s="207" t="s">
         <v>348</v>
       </c>
-      <c r="E4" s="198"/>
-      <c r="F4" s="198"/>
-      <c r="G4" s="198"/>
-      <c r="K4" s="199" t="s">
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="207"/>
+      <c r="K4" s="208" t="s">
         <v>351</v>
       </c>
-      <c r="L4" s="199"/>
-      <c r="M4" s="199"/>
-      <c r="N4" s="199"/>
-      <c r="R4" s="195" t="s">
+      <c r="L4" s="208"/>
+      <c r="M4" s="208"/>
+      <c r="N4" s="208"/>
+      <c r="R4" s="204" t="s">
         <v>352</v>
       </c>
-      <c r="S4" s="195"/>
-      <c r="T4" s="195"/>
-      <c r="U4" s="195"/>
-      <c r="Y4" s="193" t="s">
+      <c r="S4" s="204"/>
+      <c r="T4" s="204"/>
+      <c r="U4" s="204"/>
+      <c r="Y4" s="202" t="s">
         <v>353</v>
       </c>
-      <c r="Z4" s="193"/>
-      <c r="AA4" s="193"/>
-      <c r="AB4" s="193"/>
-      <c r="AF4" s="194" t="s">
+      <c r="Z4" s="202"/>
+      <c r="AA4" s="202"/>
+      <c r="AB4" s="202"/>
+      <c r="AF4" s="203" t="s">
         <v>354</v>
       </c>
-      <c r="AG4" s="194"/>
-      <c r="AH4" s="194"/>
-      <c r="AI4" s="194"/>
+      <c r="AG4" s="203"/>
+      <c r="AH4" s="203"/>
+      <c r="AI4" s="203"/>
     </row>
     <row r="5" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C5" s="115" t="s">
@@ -43211,40 +43211,40 @@
     </row>
     <row r="62" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C62" s="100"/>
-      <c r="D62" s="196" t="s">
+      <c r="D62" s="205" t="s">
         <v>356</v>
       </c>
-      <c r="E62" s="196"/>
-      <c r="F62" s="196"/>
-      <c r="G62" s="196"/>
+      <c r="E62" s="205"/>
+      <c r="F62" s="205"/>
+      <c r="G62" s="205"/>
       <c r="J62" s="100"/>
-      <c r="K62" s="197" t="s">
+      <c r="K62" s="206" t="s">
         <v>357</v>
       </c>
-      <c r="L62" s="197"/>
-      <c r="M62" s="197"/>
-      <c r="N62" s="197"/>
+      <c r="L62" s="206"/>
+      <c r="M62" s="206"/>
+      <c r="N62" s="206"/>
       <c r="Q62" s="100"/>
-      <c r="R62" s="195" t="s">
+      <c r="R62" s="204" t="s">
         <v>358</v>
       </c>
-      <c r="S62" s="195"/>
-      <c r="T62" s="195"/>
-      <c r="U62" s="195"/>
+      <c r="S62" s="204"/>
+      <c r="T62" s="204"/>
+      <c r="U62" s="204"/>
       <c r="X62" s="100"/>
-      <c r="Y62" s="193" t="s">
+      <c r="Y62" s="202" t="s">
         <v>359</v>
       </c>
-      <c r="Z62" s="193"/>
-      <c r="AA62" s="193"/>
-      <c r="AB62" s="193"/>
+      <c r="Z62" s="202"/>
+      <c r="AA62" s="202"/>
+      <c r="AB62" s="202"/>
       <c r="AE62" s="100"/>
-      <c r="AF62" s="194" t="s">
+      <c r="AF62" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="AG62" s="194"/>
-      <c r="AH62" s="194"/>
-      <c r="AI62" s="194"/>
+      <c r="AG62" s="203"/>
+      <c r="AH62" s="203"/>
+      <c r="AI62" s="203"/>
     </row>
     <row r="63" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C63" s="100" t="s">
@@ -47270,10 +47270,10 @@
     <mergeCell ref="K4:N4"/>
   </mergeCells>
   <conditionalFormatting sqref="K63:N63">
-    <cfRule type="uniqueValues" dxfId="1" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="34" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q120:T120">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="33" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -47776,7 +47776,7 @@
   <dimension ref="C6:N58"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48956,64 +48956,64 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="193" t="s">
         <v>371</v>
       </c>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
+      <c r="C5" s="193"/>
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="193"/>
     </row>
     <row r="6" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="E6" s="200" t="s">
+      <c r="E6" s="209" t="s">
         <v>372</v>
       </c>
-      <c r="F6" s="200"/>
-      <c r="I6" s="177" t="s">
+      <c r="F6" s="209"/>
+      <c r="I6" s="193" t="s">
         <v>398</v>
       </c>
-      <c r="J6" s="177"/>
-      <c r="L6" s="177" t="s">
+      <c r="J6" s="193"/>
+      <c r="L6" s="193" t="s">
         <v>393</v>
       </c>
-      <c r="M6" s="177"/>
-      <c r="N6" s="177"/>
-      <c r="O6" s="177"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
       <c r="R6" t="s">
         <v>408</v>
       </c>
-      <c r="Y6" s="177" t="s">
+      <c r="Y6" s="193" t="s">
         <v>413</v>
       </c>
-      <c r="Z6" s="177"/>
-      <c r="AA6" s="177"/>
-      <c r="AB6" s="177"/>
-      <c r="AC6" s="177"/>
-      <c r="AD6" s="177"/>
-      <c r="AG6" s="177" t="s">
+      <c r="Z6" s="193"/>
+      <c r="AA6" s="193"/>
+      <c r="AB6" s="193"/>
+      <c r="AC6" s="193"/>
+      <c r="AD6" s="193"/>
+      <c r="AG6" s="193" t="s">
         <v>430</v>
       </c>
-      <c r="AH6" s="177"/>
-      <c r="AI6" s="177"/>
-      <c r="AJ6" s="177"/>
-      <c r="AK6" s="177"/>
-      <c r="AL6" s="177"/>
-      <c r="AM6" s="177"/>
-      <c r="AN6" s="177"/>
-      <c r="AO6" s="177"/>
+      <c r="AH6" s="193"/>
+      <c r="AI6" s="193"/>
+      <c r="AJ6" s="193"/>
+      <c r="AK6" s="193"/>
+      <c r="AL6" s="193"/>
+      <c r="AM6" s="193"/>
+      <c r="AN6" s="193"/>
+      <c r="AO6" s="193"/>
     </row>
     <row r="7" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="191" t="s">
+      <c r="B7" s="200" t="s">
         <v>376</v>
       </c>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="200" t="s">
         <v>373</v>
       </c>
-      <c r="D7" s="175" t="s">
+      <c r="D7" s="191" t="s">
         <v>374</v>
       </c>
-      <c r="E7" s="175"/>
-      <c r="F7" s="191" t="s">
+      <c r="E7" s="191"/>
+      <c r="F7" s="200" t="s">
         <v>375</v>
       </c>
       <c r="J7" t="s">
@@ -49024,25 +49024,25 @@
       </c>
     </row>
     <row r="8" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B8" s="191"/>
-      <c r="C8" s="191"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="200"/>
       <c r="D8" s="120" t="s">
         <v>377</v>
       </c>
       <c r="E8" s="120" t="s">
         <v>378</v>
       </c>
-      <c r="F8" s="191"/>
+      <c r="F8" s="200"/>
       <c r="I8" s="4" t="s">
         <v>399</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="N8" s="200" t="s">
+      <c r="N8" s="209" t="s">
         <v>394</v>
       </c>
-      <c r="O8" s="200"/>
+      <c r="O8" s="209"/>
       <c r="R8" s="124" t="s">
         <v>376</v>
       </c>
@@ -49796,13 +49796,13 @@
       </c>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="200" t="s">
         <v>380</v>
       </c>
-      <c r="C21" s="175" t="s">
+      <c r="C21" s="191" t="s">
         <v>381</v>
       </c>
-      <c r="D21" s="175"/>
+      <c r="D21" s="191"/>
       <c r="L21" s="103">
         <v>2015</v>
       </c>
@@ -49832,7 +49832,7 @@
       </c>
     </row>
     <row r="22" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B22" s="191"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="103" t="s">
         <v>384</v>
       </c>
@@ -49953,10 +49953,10 @@
     </row>
     <row r="27" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B27" s="98"/>
-      <c r="AG27" s="175" t="s">
+      <c r="AG27" s="191" t="s">
         <v>21</v>
       </c>
-      <c r="AH27" s="175"/>
+      <c r="AH27" s="191"/>
       <c r="AI27" s="4">
         <f>SUM(AI20:AI26)</f>
         <v>443208</v>
@@ -49971,16 +49971,16 @@
       </c>
     </row>
     <row r="28" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B28" s="191" t="s">
+      <c r="B28" s="200" t="s">
         <v>382</v>
       </c>
-      <c r="C28" s="175" t="s">
+      <c r="C28" s="191" t="s">
         <v>383</v>
       </c>
-      <c r="D28" s="175"/>
+      <c r="D28" s="191"/>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B29" s="191"/>
+      <c r="B29" s="200"/>
       <c r="C29" s="103" t="s">
         <v>384</v>
       </c>
@@ -50054,22 +50054,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Y6:AD6"/>
-    <mergeCell ref="AG6:AO6"/>
-    <mergeCell ref="AG27:AH27"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="Y6:AD6"/>
+    <mergeCell ref="AG6:AO6"/>
+    <mergeCell ref="AG27:AH27"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50130,16 +50130,16 @@
       <c r="D5" t="s">
         <v>401</v>
       </c>
-      <c r="I5" s="169" t="s">
+      <c r="I5" s="176" t="s">
         <v>376</v>
       </c>
-      <c r="J5" s="201" t="s">
+      <c r="J5" s="210" t="s">
         <v>401</v>
       </c>
-      <c r="K5" s="201" t="s">
+      <c r="K5" s="210" t="s">
         <v>468</v>
       </c>
-      <c r="L5" s="201" t="s">
+      <c r="L5" s="210" t="s">
         <v>469</v>
       </c>
     </row>
@@ -50150,10 +50150,10 @@
       <c r="D6">
         <v>75.7</v>
       </c>
-      <c r="I6" s="169"/>
-      <c r="J6" s="201"/>
-      <c r="K6" s="201"/>
-      <c r="L6" s="201"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="210"/>
+      <c r="K6" s="210"/>
+      <c r="L6" s="210"/>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7">
@@ -50277,20 +50277,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="176" t="s">
         <v>456</v>
       </c>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
-      <c r="H4" s="169"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+      <c r="H4" s="176"/>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="203" t="s">
+      <c r="G5" s="212" t="s">
         <v>461</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="212"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D6" s="138">
@@ -50346,7 +50346,7 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="202" t="s">
+      <c r="C9" s="211" t="s">
         <v>459</v>
       </c>
       <c r="D9" s="4">
@@ -50364,7 +50364,7 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="202"/>
+      <c r="C10" s="211"/>
       <c r="D10" s="4">
         <v>3.1</v>
       </c>
@@ -50382,23 +50382,23 @@
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="177" t="s">
+      <c r="C13" s="193" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="177"/>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="177"/>
-      <c r="J13" s="177"/>
-      <c r="K13" s="177"/>
+      <c r="D13" s="193"/>
+      <c r="E13" s="193"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="193"/>
+      <c r="H13" s="193"/>
+      <c r="I13" s="193"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="193"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="J14" s="203" t="s">
+      <c r="J14" s="212" t="s">
         <v>465</v>
       </c>
-      <c r="K14" s="203"/>
+      <c r="K14" s="212"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D15" s="138">
@@ -51398,7 +51398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A86756-A0D8-4A2F-A14A-6814D605B7C6}">
   <dimension ref="C3:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -51417,17 +51417,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
-      <c r="J3" s="171"/>
-      <c r="K3" s="171"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="180"/>
+      <c r="K3" s="180"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
@@ -52085,7 +52085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7723E276-68B9-40AE-A7CE-7D9E635C51B5}">
   <dimension ref="C1:X118"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="O86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P102" sqref="P102"/>
     </sheetView>
   </sheetViews>
@@ -52110,32 +52110,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="182" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="182"/>
+      <c r="L1" s="182"/>
+      <c r="M1" s="182"/>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D3">
@@ -52960,50 +52960,50 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D31" s="174" t="s">
+      <c r="D31" s="183" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
-      <c r="H31" s="174"/>
-      <c r="I31" s="174"/>
-      <c r="J31" s="174"/>
-      <c r="K31" s="174"/>
-      <c r="L31" s="174"/>
-      <c r="M31" s="174"/>
-      <c r="P31" s="173" t="s">
+      <c r="E31" s="183"/>
+      <c r="F31" s="183"/>
+      <c r="G31" s="183"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="183"/>
+      <c r="J31" s="183"/>
+      <c r="K31" s="183"/>
+      <c r="L31" s="183"/>
+      <c r="M31" s="183"/>
+      <c r="P31" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="Q31" s="173"/>
-      <c r="R31" s="173"/>
-      <c r="S31" s="173"/>
-      <c r="T31" s="173"/>
-      <c r="U31" s="173"/>
-      <c r="V31" s="173"/>
-      <c r="W31" s="173"/>
-      <c r="X31" s="173"/>
+      <c r="Q31" s="182"/>
+      <c r="R31" s="182"/>
+      <c r="S31" s="182"/>
+      <c r="T31" s="182"/>
+      <c r="U31" s="182"/>
+      <c r="V31" s="182"/>
+      <c r="W31" s="182"/>
+      <c r="X31" s="182"/>
     </row>
     <row r="32" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D32" s="174"/>
-      <c r="E32" s="174"/>
-      <c r="F32" s="174"/>
-      <c r="G32" s="174"/>
-      <c r="H32" s="174"/>
-      <c r="I32" s="174"/>
-      <c r="J32" s="174"/>
-      <c r="K32" s="174"/>
-      <c r="L32" s="174"/>
-      <c r="M32" s="174"/>
-      <c r="P32" s="173"/>
-      <c r="Q32" s="173"/>
-      <c r="R32" s="173"/>
-      <c r="S32" s="173"/>
-      <c r="T32" s="173"/>
-      <c r="U32" s="173"/>
-      <c r="V32" s="173"/>
-      <c r="W32" s="173"/>
-      <c r="X32" s="173"/>
+      <c r="D32" s="183"/>
+      <c r="E32" s="183"/>
+      <c r="F32" s="183"/>
+      <c r="G32" s="183"/>
+      <c r="H32" s="183"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="183"/>
+      <c r="K32" s="183"/>
+      <c r="L32" s="183"/>
+      <c r="M32" s="183"/>
+      <c r="P32" s="182"/>
+      <c r="Q32" s="182"/>
+      <c r="R32" s="182"/>
+      <c r="S32" s="182"/>
+      <c r="T32" s="182"/>
+      <c r="U32" s="182"/>
+      <c r="V32" s="182"/>
+      <c r="W32" s="182"/>
+      <c r="X32" s="182"/>
     </row>
     <row r="33" spans="3:24" x14ac:dyDescent="0.25">
       <c r="D33">
@@ -54094,17 +54094,17 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P53" s="172" t="s">
+      <c r="P53" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="Q53" s="172"/>
-      <c r="R53" s="172"/>
-      <c r="S53" s="172"/>
-      <c r="T53" s="172"/>
-      <c r="U53" s="172"/>
-      <c r="V53" s="172"/>
-      <c r="W53" s="172"/>
-      <c r="X53" s="172"/>
+      <c r="Q53" s="181"/>
+      <c r="R53" s="181"/>
+      <c r="S53" s="181"/>
+      <c r="T53" s="181"/>
+      <c r="U53" s="181"/>
+      <c r="V53" s="181"/>
+      <c r="W53" s="181"/>
+      <c r="X53" s="181"/>
     </row>
     <row r="54" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C54">
@@ -54140,15 +54140,15 @@
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="P54" s="172"/>
-      <c r="Q54" s="172"/>
-      <c r="R54" s="172"/>
-      <c r="S54" s="172"/>
-      <c r="T54" s="172"/>
-      <c r="U54" s="172"/>
-      <c r="V54" s="172"/>
-      <c r="W54" s="172"/>
-      <c r="X54" s="172"/>
+      <c r="P54" s="181"/>
+      <c r="Q54" s="181"/>
+      <c r="R54" s="181"/>
+      <c r="S54" s="181"/>
+      <c r="T54" s="181"/>
+      <c r="U54" s="181"/>
+      <c r="V54" s="181"/>
+      <c r="W54" s="181"/>
+      <c r="X54" s="181"/>
     </row>
     <row r="55" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C55">
@@ -54853,28 +54853,28 @@
       <c r="W72" s="19"/>
     </row>
     <row r="78" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D78" s="172" t="s">
+      <c r="D78" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="E78" s="172"/>
-      <c r="F78" s="172"/>
-      <c r="G78" s="172"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="172"/>
-      <c r="J78" s="172"/>
-      <c r="K78" s="172"/>
-      <c r="L78" s="172"/>
+      <c r="E78" s="181"/>
+      <c r="F78" s="181"/>
+      <c r="G78" s="181"/>
+      <c r="H78" s="181"/>
+      <c r="I78" s="181"/>
+      <c r="J78" s="181"/>
+      <c r="K78" s="181"/>
+      <c r="L78" s="181"/>
     </row>
     <row r="79" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D79" s="172"/>
-      <c r="E79" s="172"/>
-      <c r="F79" s="172"/>
-      <c r="G79" s="172"/>
-      <c r="H79" s="172"/>
-      <c r="I79" s="172"/>
-      <c r="J79" s="172"/>
-      <c r="K79" s="172"/>
-      <c r="L79" s="172"/>
+      <c r="D79" s="181"/>
+      <c r="E79" s="181"/>
+      <c r="F79" s="181"/>
+      <c r="G79" s="181"/>
+      <c r="H79" s="181"/>
+      <c r="I79" s="181"/>
+      <c r="J79" s="181"/>
+      <c r="K79" s="181"/>
+      <c r="L79" s="181"/>
     </row>
     <row r="80" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
@@ -55473,28 +55473,28 @@
       </c>
     </row>
     <row r="99" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D99" s="172" t="s">
+      <c r="D99" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="E99" s="172"/>
-      <c r="F99" s="172"/>
-      <c r="G99" s="172"/>
-      <c r="H99" s="172"/>
-      <c r="I99" s="172"/>
-      <c r="J99" s="172"/>
-      <c r="K99" s="172"/>
-      <c r="L99" s="172"/>
+      <c r="E99" s="181"/>
+      <c r="F99" s="181"/>
+      <c r="G99" s="181"/>
+      <c r="H99" s="181"/>
+      <c r="I99" s="181"/>
+      <c r="J99" s="181"/>
+      <c r="K99" s="181"/>
+      <c r="L99" s="181"/>
     </row>
     <row r="100" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D100" s="172"/>
-      <c r="E100" s="172"/>
-      <c r="F100" s="172"/>
-      <c r="G100" s="172"/>
-      <c r="H100" s="172"/>
-      <c r="I100" s="172"/>
-      <c r="J100" s="172"/>
-      <c r="K100" s="172"/>
-      <c r="L100" s="172"/>
+      <c r="D100" s="181"/>
+      <c r="E100" s="181"/>
+      <c r="F100" s="181"/>
+      <c r="G100" s="181"/>
+      <c r="H100" s="181"/>
+      <c r="I100" s="181"/>
+      <c r="J100" s="181"/>
+      <c r="K100" s="181"/>
+      <c r="L100" s="181"/>
     </row>
     <row r="101" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D101" t="s">

</xml_diff>